<commit_message>
feat: cambios en el excel default de constancia de visita.
</commit_message>
<xml_diff>
--- a/files/Constancia visita/Constancia de Visita.xlsx
+++ b/files/Constancia visita/Constancia de Visita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\back-proteccion\api\files\Constancia visita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660582E4-5B0C-419E-AC7E-2DF47CA9A086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C36EAA-3C57-42F5-8C8D-99A7AA496AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="4272" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constancia de Visita" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t xml:space="preserve"> Cant. Trab.</t>
   </si>
@@ -564,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -611,9 +611,177 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,200 +797,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,8 +1315,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:L49"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1337,43 +1328,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="41" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
       <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="47">
+      <c r="K2" s="67">
         <v>2</v>
       </c>
-      <c r="L2" s="48"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="66"/>
       <c r="J3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="K3" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="50"/>
+      <c r="L3" s="70"/>
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,122 +1382,122 @@
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="58"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="29"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="28" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="32" t="s">
+      <c r="J8" s="51"/>
+      <c r="K8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="29"/>
+      <c r="L8" s="51"/>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="31"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="28" t="s">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="28" t="s">
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="28" t="s">
+      <c r="J10" s="51"/>
+      <c r="K10" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="29"/>
+      <c r="L10" s="51"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1523,34 +1514,34 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="29"/>
     </row>
     <row r="15" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1567,65 +1558,65 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="14"/>
       <c r="G19" s="11" t="s">
         <v>27</v>
@@ -1637,13 +1628,13 @@
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="14"/>
       <c r="G20" s="11" t="s">
         <v>28</v>
@@ -1655,557 +1646,555 @@
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="24"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="21"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="77"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="77"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="69"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="71"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+    </row>
+    <row r="25" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="78"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="80"/>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="72"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="74"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="83"/>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75"/>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="77"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="83"/>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="75"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="77"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="83"/>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="74"/>
+      <c r="A29" s="81"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="83"/>
     </row>
     <row r="30" spans="1:12" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
     </row>
     <row r="31" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="67"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
     </row>
     <row r="32" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="36"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="78"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="80"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="82"/>
-      <c r="H34" s="82"/>
-      <c r="I34" s="82"/>
-      <c r="J34" s="82"/>
-      <c r="K34" s="82"/>
-      <c r="L34" s="83"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="21"/>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="81"/>
-      <c r="B35" s="82"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="82"/>
-      <c r="K35" s="82"/>
-      <c r="L35" s="83"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="21"/>
     </row>
     <row r="36" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="82"/>
-      <c r="L36" s="83"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="21"/>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="81"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="82"/>
-      <c r="L37" s="83"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="21"/>
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="81"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82"/>
-      <c r="J38" s="82"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="83"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="21"/>
     </row>
     <row r="39" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="81"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="83"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="82"/>
-      <c r="I40" s="82"/>
-      <c r="J40" s="82"/>
-      <c r="K40" s="82"/>
-      <c r="L40" s="83"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="21"/>
     </row>
     <row r="41" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="81"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="82"/>
-      <c r="G41" s="82"/>
-      <c r="H41" s="82"/>
-      <c r="I41" s="82"/>
-      <c r="J41" s="82"/>
-      <c r="K41" s="82"/>
-      <c r="L41" s="83"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="21"/>
     </row>
     <row r="42" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="81"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="82"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="82"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="83"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="21"/>
     </row>
     <row r="43" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="81"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="82"/>
-      <c r="K43" s="82"/>
-      <c r="L43" s="83"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="21"/>
     </row>
     <row r="44" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="81"/>
-      <c r="B44" s="82"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="82"/>
-      <c r="K44" s="82"/>
-      <c r="L44" s="83"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="21"/>
     </row>
     <row r="45" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="81"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="83"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="21"/>
     </row>
     <row r="46" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="81"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="83"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="21"/>
     </row>
     <row r="47" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="81"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="83"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="21"/>
     </row>
     <row r="48" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="81"/>
-      <c r="B48" s="82"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="83"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="21"/>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="84"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="86"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="24"/>
     </row>
     <row r="50" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="60" t="s">
+      <c r="A50" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="61"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="62"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="46"/>
     </row>
     <row r="51" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="63" t="s">
+      <c r="A52" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="28" t="s">
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="29"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="51"/>
     </row>
     <row r="53" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54" t="s">
+      <c r="A53" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="54" t="s">
+      <c r="B53" s="56"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="55"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="51"/>
-      <c r="K53" s="51"/>
-      <c r="L53" s="51"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
     </row>
     <row r="54" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="54" t="s">
+      <c r="B54" s="56"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H54" s="55"/>
-      <c r="I54" s="52" t="s">
+      <c r="H54" s="56"/>
+      <c r="I54" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="J54" s="52"/>
-      <c r="K54" s="52"/>
-      <c r="L54" s="52"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="53"/>
     </row>
     <row r="55" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="55" t="s">
+      <c r="A55" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="55" t="s">
+      <c r="B55" s="56"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="H55" s="55"/>
-      <c r="I55" s="52" t="s">
+      <c r="H55" s="56"/>
+      <c r="I55" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="J55" s="52"/>
-      <c r="K55" s="52"/>
-      <c r="L55" s="52"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
     </row>
     <row r="56" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="55" t="s">
+      <c r="A56" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="55"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="55" t="s">
+      <c r="B56" s="56"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="55"/>
-      <c r="I56" s="53" t="s">
+      <c r="H56" s="56"/>
+      <c r="I56" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
+      <c r="J56" s="54"/>
+      <c r="K56" s="54"/>
+      <c r="L56" s="54"/>
     </row>
     <row r="57" spans="1:12" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="59"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="59"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="59"/>
-      <c r="K57" s="59"/>
-      <c r="L57" s="59"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
     </row>
     <row r="58" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2238,23 +2227,44 @@
     <row r="86" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="87" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="A33:L49"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="A14:L14"/>
+  <mergeCells count="64">
+    <mergeCell ref="A25:L29"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:I3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
     <mergeCell ref="A13:L13"/>
     <mergeCell ref="A57:L57"/>
     <mergeCell ref="A50:L50"/>
@@ -2271,42 +2281,17 @@
     <mergeCell ref="I53:L53"/>
     <mergeCell ref="I54:L54"/>
     <mergeCell ref="I55:L55"/>
-    <mergeCell ref="I56:L56"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:I3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A33:L49"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="A14:L14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
feat: actualización archivo default constancia visita.
</commit_message>
<xml_diff>
--- a/files/Constancia visita/Constancia de Visita.xlsx
+++ b/files/Constancia visita/Constancia de Visita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\back-proteccion\api\files\Constancia visita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C36EAA-3C57-42F5-8C8D-99A7AA496AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AA7002-CF7F-4DA6-88C2-E9B92FD31CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="4272" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -690,7 +690,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,6 +788,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -796,24 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,8 +1324,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:L7"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1328,43 +1337,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="61" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
       <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="67">
+      <c r="K2" s="69">
         <v>2</v>
       </c>
-      <c r="L2" s="68"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="66"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
       <c r="J3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="69" t="s">
+      <c r="K3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="70"/>
+      <c r="L3" s="72"/>
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1398,25 +1407,25 @@
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="51"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -1424,33 +1433,33 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="42"/>
+      <c r="I7" s="75"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="29"/>
     </row>
     <row r="8" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="49" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="50" t="s">
+      <c r="J8" s="53"/>
+      <c r="K8" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="51"/>
+      <c r="L8" s="53"/>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -1464,39 +1473,39 @@
       <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="49" t="s">
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="49" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="49" t="s">
+      <c r="J10" s="53"/>
+      <c r="K10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="51"/>
+      <c r="L10" s="53"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
-      <c r="B11" s="72"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="37"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="37"/>
-      <c r="I11" s="72"/>
+      <c r="I11" s="74"/>
       <c r="J11" s="37"/>
-      <c r="K11" s="72"/>
+      <c r="K11" s="74"/>
       <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1531,17 +1540,17 @@
     </row>
     <row r="14" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="29"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1558,20 +1567,20 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
@@ -1582,13 +1591,13 @@
       <c r="D17" s="34"/>
       <c r="E17" s="35"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
       <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1672,116 +1681,116 @@
       <c r="D22" s="34"/>
       <c r="E22" s="35"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="77"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="86"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="77"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="80"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="78"/>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="83"/>
+      <c r="A26" s="79"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="81"/>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="82"/>
-      <c r="L27" s="83"/>
+      <c r="A27" s="79"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="81"/>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="82"/>
-      <c r="K28" s="82"/>
-      <c r="L28" s="83"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="81"/>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="81"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="82"/>
-      <c r="K29" s="82"/>
-      <c r="L29" s="83"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="81"/>
     </row>
     <row r="30" spans="1:12" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
@@ -2070,131 +2079,131 @@
       <c r="L49" s="24"/>
     </row>
     <row r="50" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="46"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="48"/>
     </row>
     <row r="51" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="49" t="s">
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="51"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="53"/>
     </row>
     <row r="53" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="55" t="s">
+      <c r="A53" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="56"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="55" t="s">
+      <c r="B53" s="58"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="56"/>
-      <c r="I53" s="52"/>
-      <c r="J53" s="52"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="54"/>
+      <c r="J53" s="54"/>
+      <c r="K53" s="54"/>
+      <c r="L53" s="54"/>
     </row>
     <row r="54" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="55" t="s">
+      <c r="A54" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="55" t="s">
+      <c r="B54" s="58"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H54" s="56"/>
-      <c r="I54" s="53" t="s">
+      <c r="H54" s="58"/>
+      <c r="I54" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="J54" s="53"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="53"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
     </row>
     <row r="55" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="56"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="56" t="s">
+      <c r="B55" s="58"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="H55" s="56"/>
-      <c r="I55" s="53" t="s">
+      <c r="H55" s="58"/>
+      <c r="I55" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="53"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
     </row>
     <row r="56" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
+      <c r="A56" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="56" t="s">
+      <c r="B56" s="58"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="56"/>
-      <c r="I56" s="54" t="s">
+      <c r="H56" s="58"/>
+      <c r="I56" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="J56" s="54"/>
-      <c r="K56" s="54"/>
-      <c r="L56" s="54"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="56"/>
     </row>
     <row r="57" spans="1:12" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="43"/>
+      <c r="A57" s="45"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
+      <c r="L57" s="45"/>
     </row>
     <row r="58" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2228,24 +2237,6 @@
     <row r="87" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="A25:L29"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:I3"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="G17:K17"/>
@@ -2260,12 +2251,24 @@
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A9:H9"/>
-    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="G54:H54"/>
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:I3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A25:L29"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="A57:L57"/>
     <mergeCell ref="A50:L50"/>
     <mergeCell ref="A52:F52"/>
@@ -2281,6 +2284,7 @@
     <mergeCell ref="I53:L53"/>
     <mergeCell ref="I54:L54"/>
     <mergeCell ref="I55:L55"/>
+    <mergeCell ref="I56:L56"/>
     <mergeCell ref="A33:L49"/>
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="I9:J9"/>
@@ -2292,6 +2296,11 @@
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
feat: actualizo constancia de visita
</commit_message>
<xml_diff>
--- a/files/Constancia visita/Constancia de Visita.xlsx
+++ b/files/Constancia visita/Constancia de Visita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\back-proteccion\api\files\Constancia visita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AA7002-CF7F-4DA6-88C2-E9B92FD31CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D749AFDD-C423-4314-8D20-253782A91DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="4272" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,6 +611,153 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -647,12 +794,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -662,21 +803,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -697,132 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,8 +1324,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:L29"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="118" zoomScaleNormal="170" zoomScaleSheetLayoutView="118" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1337,43 +1337,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="63" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="69">
+      <c r="K2" s="16">
         <v>2</v>
       </c>
-      <c r="L2" s="70"/>
+      <c r="L2" s="17"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="K3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="19"/>
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,122 +1391,122 @@
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="76"/>
     </row>
     <row r="6" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="51" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="53"/>
-      <c r="K8" s="52" t="s">
+      <c r="J8" s="25"/>
+      <c r="K8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="53"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="51" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="51" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="51" t="s">
+      <c r="J10" s="25"/>
+      <c r="K10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="53"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="37"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1523,34 +1523,34 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="76"/>
     </row>
     <row r="14" spans="1:13" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:13" ht="6.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1567,65 +1567,65 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="83" t="s">
+      <c r="A16" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="73" t="s">
+      <c r="G17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="14"/>
       <c r="G19" s="11" t="s">
         <v>27</v>
@@ -1637,13 +1637,13 @@
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="14"/>
       <c r="G20" s="11" t="s">
         <v>28</v>
@@ -1655,555 +1655,555 @@
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="84" t="s">
+      <c r="G22" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="85"/>
-      <c r="K22" s="86"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="55"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="86"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="82"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="76"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="78"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="47"/>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="81"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="50"/>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="81"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="50"/>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="81"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="50"/>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="80"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="81"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
     </row>
     <row r="30" spans="1:12" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="83"/>
     </row>
     <row r="31" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="82"/>
     </row>
     <row r="32" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="32"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="79"/>
     </row>
     <row r="33" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="18"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="67"/>
     </row>
     <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="21"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="70"/>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="21"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="70"/>
     </row>
     <row r="36" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="21"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="70"/>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="21"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="70"/>
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="21"/>
+      <c r="A38" s="68"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="70"/>
     </row>
     <row r="39" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="21"/>
+      <c r="A39" s="68"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="70"/>
     </row>
     <row r="40" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="21"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="70"/>
     </row>
     <row r="41" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="21"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="69"/>
+      <c r="K41" s="69"/>
+      <c r="L41" s="70"/>
     </row>
     <row r="42" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="21"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
+      <c r="K42" s="69"/>
+      <c r="L42" s="70"/>
     </row>
     <row r="43" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="21"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="70"/>
     </row>
     <row r="44" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="21"/>
+      <c r="A44" s="68"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="70"/>
     </row>
     <row r="45" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="21"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="70"/>
     </row>
     <row r="46" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="21"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="70"/>
     </row>
     <row r="47" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="21"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="70"/>
     </row>
     <row r="48" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="21"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="69"/>
+      <c r="L48" s="70"/>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="72"/>
+      <c r="K49" s="72"/>
+      <c r="L49" s="73"/>
     </row>
     <row r="50" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="48"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="59"/>
     </row>
     <row r="51" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" s="6" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="51" t="s">
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="53"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="25"/>
     </row>
     <row r="53" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="57" t="s">
+      <c r="B53" s="33"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="58"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
     </row>
     <row r="54" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="58"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="57" t="s">
+      <c r="B54" s="33"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H54" s="58"/>
-      <c r="I54" s="55" t="s">
+      <c r="H54" s="33"/>
+      <c r="I54" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="J54" s="55"/>
-      <c r="K54" s="55"/>
-      <c r="L54" s="55"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="63"/>
     </row>
     <row r="55" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="58" t="s">
+      <c r="A55" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="58"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="58" t="s">
+      <c r="B55" s="33"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H55" s="58"/>
-      <c r="I55" s="55" t="s">
+      <c r="H55" s="33"/>
+      <c r="I55" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="J55" s="55"/>
-      <c r="K55" s="55"/>
-      <c r="L55" s="55"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
     </row>
     <row r="56" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="58" t="s">
+      <c r="A56" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="58"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="58" t="s">
+      <c r="B56" s="33"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="58"/>
-      <c r="I56" s="56" t="s">
+      <c r="H56" s="33"/>
+      <c r="I56" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="J56" s="56"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
+      <c r="J56" s="64"/>
+      <c r="K56" s="64"/>
+      <c r="L56" s="64"/>
     </row>
     <row r="57" spans="1:12" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
+      <c r="A57" s="56"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
     </row>
     <row r="58" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:12" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2237,6 +2237,54 @@
     <row r="87" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A33:L49"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A57:L57"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="G52:L52"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="I53:L53"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:I3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A25:L29"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="G17:K17"/>
@@ -2253,54 +2301,6 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:I3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A25:L29"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="A57:L57"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="G52:L52"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I55:L55"/>
-    <mergeCell ref="I56:L56"/>
-    <mergeCell ref="A33:L49"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>